<commit_message>
Write results to file
</commit_message>
<xml_diff>
--- a/MetricsCalculators/Metric-Joinpoints.xlsx
+++ b/MetricsCalculators/Metric-Joinpoints.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Validation" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Results" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Internal Validation" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="External Val" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="307">
   <si>
     <t xml:space="preserve">*</t>
   </si>
@@ -881,6 +881,9 @@
     <t xml:space="preserve">Using only number of methods</t>
   </si>
   <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
     <t xml:space="preserve">The difference in number of semicolons is expected
 There is a problem with class.parent</t>
   </si>
@@ -891,9 +894,6 @@
     <t xml:space="preserve">LOC*</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
     <t xml:space="preserve">How to properly calculate LOC?</t>
   </si>
   <si>
@@ -990,9 +990,6 @@
     <t xml:space="preserve">stars:&gt;5000 size:&lt;1000 language:Java</t>
   </si>
   <si>
-    <t xml:space="preserve">Metrics</t>
-  </si>
-  <si>
     <t xml:space="preserve">LARA(have to clean code)</t>
   </si>
   <si>
@@ -1002,7 +999,99 @@
     <t xml:space="preserve">Sonarqube: I could only find the implementation for js</t>
   </si>
   <si>
+    <t xml:space="preserve">Execution Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pbeans (50 classes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of immediate sub-classes of a class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maximum inheritance path from the class to the root class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA, however for Java since every object extends Object, it has a minimum of 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of methods in class + remote methods directly called by methods of the class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA (diff results, I don’t understand this results)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of methods, including inherited ones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of methods defined in class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of cyclomatic complexity of all methods/functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCOM94 aka lcom1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lcom4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate for every att, the percetange number of methods that used it. Average the percentages and subtract from 100%. lower is better.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.686.2543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Coupling Between Object classes metric represents the number of classes coupled to a given class. This coupling can happen throuhg:
+    method call
+    class extends
+    properties or parameters
+    method arguments, or return types
+    variables in methods
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A class is coupled to another if it uses:
+   A uses a attribute or method of another or vice-versa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A class is coupled to another if it uses:
+   A uses a type, attribute or method of another</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of methods, I think for c++ it counts the default constructor, copy constructor and destructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of semicolons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA, diff results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of methods cyclomatic comp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg cyclomatic comp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analizo uses Doxygen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To calculate CC it counts keywords</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1427,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1433,6 +1522,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="34" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3489,7 +3582,7 @@
   <dimension ref="A4:K129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3943,6 +4036,9 @@
       <c r="I32" s="0" t="s">
         <v>198</v>
       </c>
+      <c r="J32" s="0" t="n">
+        <v>55</v>
+      </c>
       <c r="K32" s="0" t="s">
         <v>199</v>
       </c>
@@ -4040,10 +4136,13 @@
         <v>3152</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>2433</v>
+        <v>2618</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>77</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>2581</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4566,10 +4665,10 @@
   <dimension ref="A3:Y79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.63"/>
@@ -4939,6 +5038,9 @@
       <c r="I11" s="5" t="n">
         <v>4</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>239</v>
+      </c>
       <c r="L11" s="5" t="n">
         <v>3</v>
       </c>
@@ -4999,7 +5101,7 @@
         <v>25</v>
       </c>
       <c r="U12" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5168,7 +5270,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0</v>
@@ -5209,7 +5311,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>27</v>
@@ -5230,7 +5332,7 @@
         <v>12</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L18" s="5" t="n">
         <v>22</v>
@@ -5819,7 +5921,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -5836,7 +5938,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>22</v>
@@ -6345,7 +6447,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -6363,7 +6465,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -6694,7 +6796,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B78" s="5" t="n">
         <v>0</v>
@@ -6735,7 +6837,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B79" s="5" t="n">
         <v>23</v>
@@ -6790,15 +6892,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C59"/>
+  <dimension ref="A2:L79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="37.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="33.41"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6806,15 +6913,17 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>275</v>
-      </c>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>158</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6960,7 +7069,7 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6968,16 +7077,20 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>158</v>
+        <v>279</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>187</v>
@@ -6988,113 +7101,137 @@
         <v>189</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="5" t="n">
+        <v>4954.09965515137</v>
+      </c>
       <c r="C40" s="0" t="n">
         <v>1588</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="5" t="n">
+        <v>264.167785644531</v>
+      </c>
       <c r="C41" s="0" t="n">
         <v>1577</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="5"/>
+      <c r="B42" s="5" t="n">
+        <v>613.927841186523</v>
+      </c>
       <c r="C42" s="0" t="n">
         <v>3644</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="5"/>
+      <c r="B43" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C43" s="0" t="n">
         <v>1569</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="5" t="n">
+        <v>40291.5477752686</v>
+      </c>
       <c r="C44" s="0" t="n">
         <v>16433</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="5"/>
+      <c r="B45" s="5" t="n">
+        <v>1859.90333557129</v>
+      </c>
       <c r="C45" s="0" t="n">
         <v>4701</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="5" t="n">
+        <v>182.628631591797</v>
+      </c>
       <c r="C46" s="0" t="n">
         <v>1588</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="5"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C48" s="0" t="n">
         <v>1618</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C49" s="0" t="n">
         <v>3312</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C50" s="0" t="n">
         <v>1634</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="5" t="n">
+        <v>6480.69381713867</v>
+      </c>
       <c r="C51" s="0" t="n">
         <v>17267</v>
       </c>
@@ -7108,11 +7245,13 @@
         <v>8792</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="5"/>
+      <c r="B53" s="5" t="n">
+        <v>7063.86566162109</v>
+      </c>
       <c r="C53" s="0" t="n">
         <v>1571</v>
       </c>
@@ -7122,12 +7261,217 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H60" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G63" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G64" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G65" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G66" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="176.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="I67" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G68" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G69" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G72" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G73" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G74" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I78" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I79" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L66" r:id="rId1" display="*http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.686.2543"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Clean dead code and now display total time and time per class
</commit_message>
<xml_diff>
--- a/MetricsCalculators/Metric-Joinpoints.xlsx
+++ b/MetricsCalculators/Metric-Joinpoints.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="metric-jp" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Validation" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Results" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Internal Validation" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="External Val" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Validation-Results" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Results-LOC" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Results-Time" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="312">
   <si>
     <t xml:space="preserve">*</t>
   </si>
@@ -875,94 +876,65 @@
     <t xml:space="preserve">Transaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Fix super calls in Cpp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using only number of methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The difference in number of semicolons is expected
-There is a problem with class.parent</t>
+    <t xml:space="preserve">- The difference in LOC and SIZE1 is expected;
+- SIZE1 calculates the number of semicolons;
+- LOC gets the endline of class minus the startline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOC*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Work in progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand/Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand/Cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- In Java, every class extends Object, thats why DIT has a minimum of 1.
+- The number of constructors is different because Understands counts the default constructor, the copy constructor and the destructor
+- The difference in LOC and SIZE1 is expected;
+- The LCOM result is given as an percentage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountClassDerived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxINhereitanceTree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountDeclMethodAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SumCyclomatic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PercentLackOfCohesion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountClassCoupled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountDeclMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CountSemicolon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AvgCyclomatic</t>
   </si>
   <si>
     <t xml:space="preserve">CogniComplex*</t>
   </si>
   <si>
-    <t xml:space="preserve">LOC*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to properly calculate LOC?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HH*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Work in progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Understand/Java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Understand/Cpp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why is different</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defintions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Understand names</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountClassDerived</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Java, every class extends Object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum of all methods including inherited ones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxINhereitanceTree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of methods is different because C++, adds constructors for copy, operator =, and detructor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountDeclMethodAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCOM given as percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SumCyclomatic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PercentLackOfCohesion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountClassCoupled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountDeclMethod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The difference in number of semicolons is expected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CountSemicolon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AvgCyclomatic instead of total complexity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyclomatic/AvgCyclomatic</t>
-  </si>
-  <si>
     <t xml:space="preserve">CountLineCode</t>
   </si>
   <si>
@@ -987,55 +959,34 @@
     <t xml:space="preserve">29+14</t>
   </si>
   <si>
-    <t xml:space="preserve">stars:&gt;5000 size:&lt;1000 language:Java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LARA(have to clean code)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tool Used: cloc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonarqube: I could only find the implementation for js</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Execution Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pbeans (50 classes)</t>
+    <t xml:space="preserve">LARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of immediate sub-classes of a class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maximum inheritance path from the class to the root class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA, however for Java since every object extends Object, it has a minimum of 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of methods in class + remote methods directly called by methods of the class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as LARA (diff results, I don’t understand this results)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of methods, including inherited ones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of methods defined in class</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LARA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of immediate sub-classes of a class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same as LARA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> maximum inheritance path from the class to the root class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same as LARA, however for Java since every object extends Object, it has a minimum of 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of methods in class + remote methods directly called by methods of the class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same as LARA (diff results, I don’t understand this results)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of methods, including inherited ones.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of methods defined in class</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of cyclomatic complexity of all methods/functions</t>
@@ -1093,16 +1044,95 @@
   <si>
     <t xml:space="preserve">To calculate CC it counts keywords</t>
   </si>
+  <si>
+    <t xml:space="preserve">Analizo (only Calculate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARA (only calculate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonarqube (JAVA – visitor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who has less lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analizo (Full File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARA (Full File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Sonarqube has an implementation for every language.(1)
+- Sonarqube has a visitor for each type of node.
+- Analizo calculates another version of LCOM.
+- For Cyclomatic Complexity, Analizo uses the number of conditional statements provided by doxygen (which does not have ternary operator).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1)https://github.com/SonarSource/sonar-java/tree/ab10b6ecfaa502b96d314c66d0862714acbe400a/java-frontend/src/main/java/org/sonar/java/ast/visitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tool Used: cloc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARA Store java (6 classes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARA Store cpp (6 classes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analizo (Java)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analizo (Cpp)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Results in microsseconds (10^-6)
+- Ckjm (Java) measured with System.nanoTime();
+- Lara (JS) measured with performance.now();
+- Analizo (Perl) measured with Time::HiRes::gettimeofday();
+- Original CKJM calculated 2 extra metrics, those were removed in the fork;
+- LARA calculates in milliseconds, the ones that have 0 is because it took less and 0.5 milliseconds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total (ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elastic Search (232  classes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Elastic Search is the Java project with most stars on github (not couting guides or lists of questions/design patterns)
+-In LARA, it was compiled with incomplete classpath.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean Search (62 classes)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1258,6 +1288,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -1427,7 +1464,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1524,8 +1561,20 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="34" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2778,7 +2827,7 @@
   </sheetPr>
   <dimension ref="A3:AC73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3582,7 +3631,7 @@
   <dimension ref="A4:K129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="G60" activeCellId="0" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4662,13 +4711,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:Y79"/>
+  <dimension ref="A3:AA109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G96" activeCellId="0" sqref="G96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.63"/>
@@ -4680,6 +4729,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.86"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +4814,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -4804,6 +4854,13 @@
       <c r="S5" s="5" t="n">
         <v>0</v>
       </c>
+      <c r="U5" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -4845,6 +4902,11 @@
       <c r="S6" s="5" t="n">
         <v>0</v>
       </c>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -4886,55 +4948,59 @@
       <c r="S7" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="U7" s="0" t="s">
-        <v>237</v>
-      </c>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O8" s="5" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="P8" s="5" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="R8" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="U8" s="0" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -4974,8 +5040,13 @@
       <c r="S9" s="5" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -5015,52 +5086,54 @@
       <c r="S10" s="5" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L11" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="M11" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E11" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="H11" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I11" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="L11" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="M11" s="5" t="n">
-        <v>3</v>
-      </c>
       <c r="O11" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P11" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R11" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S11" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -5100,52 +5173,50 @@
       <c r="S12" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="U12" s="19" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U12" s="19"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="L13" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="M13" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="E13" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I13" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L13" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M13" s="5" t="n">
-        <v>5</v>
-      </c>
       <c r="O13" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P13" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R13" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S13" s="5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -5227,7 +5298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>193</v>
       </c>
@@ -5270,7 +5341,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>241</v>
+        <v>59</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>0</v>
@@ -5309,9 +5380,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B18" s="5" t="n">
         <v>27</v>
@@ -5331,9 +5402,6 @@
       <c r="I18" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="K18" s="0" t="s">
-        <v>239</v>
-      </c>
       <c r="L18" s="5" t="n">
         <v>22</v>
       </c>
@@ -5352,59 +5420,62 @@
       <c r="S18" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="U18" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+      <c r="U25" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>189</v>
       </c>
@@ -5444,17 +5515,11 @@
       <c r="S26" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="U26" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="W26" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="Y26" s="0" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA26" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>12</v>
       </c>
@@ -5494,8 +5559,15 @@
       <c r="S27" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y27" s="0" t="s">
-        <v>251</v>
+      <c r="U27" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="AA27" s="0" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5538,14 +5610,13 @@
       <c r="S28" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="U28" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="W28" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="Y28" s="0" t="s">
-        <v>254</v>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="AA28" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5588,11 +5659,13 @@
       <c r="S29" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="U29" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="Y29" s="0" t="s">
-        <v>256</v>
+      <c r="U29" s="24"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="24"/>
+      <c r="AA29" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5635,11 +5708,13 @@
       <c r="S30" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="W30" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y30" s="0" t="s">
-        <v>258</v>
+      <c r="U30" s="24"/>
+      <c r="V30" s="24"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="Y30" s="24"/>
+      <c r="AA30" s="0" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5682,8 +5757,13 @@
       <c r="S31" s="5" t="n">
         <v>66</v>
       </c>
-      <c r="Y31" s="0" t="s">
-        <v>259</v>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
+      <c r="AA31" s="0" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5726,8 +5806,13 @@
       <c r="S32" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="Y32" s="0" t="s">
-        <v>260</v>
+      <c r="U32" s="24"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="24"/>
+      <c r="AA32" s="0" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,8 +5855,8 @@
       <c r="S33" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Y33" s="0" t="s">
-        <v>261</v>
+      <c r="AA33" s="0" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,11 +5899,8 @@
       <c r="S34" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="U34" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="Y34" s="0" t="s">
-        <v>263</v>
+      <c r="AA34" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5871,9 +5953,6 @@
       <c r="P37" s="5"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
-      <c r="W37" s="0" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
@@ -5915,13 +5994,13 @@
       <c r="S38" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y38" s="0" t="s">
-        <v>265</v>
+      <c r="AA38" s="7" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -5936,9 +6015,9 @@
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>22</v>
@@ -5976,13 +6055,13 @@
       <c r="S40" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="Y40" s="0" t="s">
-        <v>266</v>
+      <c r="AA40" s="0" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6023,7 +6102,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>232</v>
       </c>
@@ -6061,7 +6140,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>12</v>
       </c>
@@ -6103,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>14</v>
       </c>
@@ -6145,7 +6224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
@@ -6187,7 +6266,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -6205,7 +6284,7 @@
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -6247,7 +6326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
         <v>28</v>
       </c>
@@ -6289,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>36</v>
       </c>
@@ -6331,7 +6410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
         <v>38</v>
       </c>
@@ -6349,7 +6428,7 @@
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
         <v>43</v>
       </c>
@@ -6367,7 +6446,7 @@
       <c r="R55" s="5"/>
       <c r="S55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
         <v>46</v>
       </c>
@@ -6385,7 +6464,7 @@
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
         <v>49</v>
       </c>
@@ -6403,7 +6482,7 @@
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
         <v>193</v>
       </c>
@@ -6445,9 +6524,9 @@
         <v>1.3333333</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -6463,9 +6542,9 @@
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -6481,51 +6560,54 @@
       <c r="R60" s="5"/>
       <c r="S60" s="5"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K61" s="4"/>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W61" s="7"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
         <v>189</v>
       </c>
@@ -6566,7 +6648,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
         <v>12</v>
       </c>
@@ -6796,7 +6878,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="B78" s="5" t="n">
         <v>0</v>
@@ -6837,31 +6919,31 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B79" s="5" t="n">
         <v>23</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="E79" s="5" t="n">
         <v>49</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="H79" s="5" t="n">
         <v>21</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="L79" s="5" t="n">
         <v>18</v>
       </c>
       <c r="M79" s="5" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="O79" s="5" t="n">
         <v>130</v>
@@ -6873,10 +6955,215 @@
         <v>34</v>
       </c>
       <c r="S79" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="163.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="96.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E94" s="5" t="s">
         <v>273</v>
       </c>
     </row>
+    <row r="95" customFormat="false" ht="243.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="539.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="184.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+    </row>
+    <row r="102" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D107" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D108" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="U5:Y10"/>
+    <mergeCell ref="U27:Y32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G95" r:id="rId1" display="*http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.686.2543"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6892,585 +7179,434 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L79"/>
+  <dimension ref="A2:J83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="37.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="33.41"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>158</v>
+        <v>289</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>290</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" s="26" t="n">
+        <f aca="false">1-C6/B6</f>
+        <v>0.0833333333333334</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="26" t="n">
+        <f aca="false">1-C7/B7</f>
+        <v>0.384615384615385</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" s="26" t="n">
+        <f aca="false">1-C8/B8</f>
+        <v>0.0666666666666667</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" s="26" t="e">
+        <f aca="false">1-C9/B9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E10" s="26" t="n">
+        <f aca="false">1-C10/B10</f>
+        <v>-0.375</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E11" s="26" t="n">
+        <f aca="false">1-C11/B11</f>
+        <v>0.12</v>
+      </c>
+      <c r="F11" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="G11" s="0" t="n">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="26" t="n">
+        <f aca="false">1-C12/B12</f>
+        <v>0.4</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="G12" s="0" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E13" s="26" t="e">
+        <f aca="false">1-C13/B13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="26" t="e">
+        <f aca="false">1-C14/B14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E15" s="26" t="e">
+        <f aca="false">1-C15/B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" s="26" t="e">
+        <f aca="false">1-C16/B16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B17" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="E17" s="26" t="n">
+        <f aca="false">1-C17/B17</f>
+        <v>-1.08333333333333</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="G17" s="0" t="n">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="E18" s="26" t="e">
+        <f aca="false">1-C18/B18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" s="26" t="e">
+        <f aca="false">1-C19/B19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>276</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>277</v>
-      </c>
-    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="5" t="n">
-        <v>4954.09965515137</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="5" t="n">
-        <v>264.167785644531</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="5" t="n">
-        <v>613.927841186523</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>3644</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="5" t="n">
-        <v>40291.5477752686</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>16433</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="5" t="n">
-        <v>1859.90333557129</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <v>4701</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="5" t="n">
-        <v>182.628631591797</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>3312</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>1634</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="B51" s="5" t="n">
-        <v>6480.69381713867</v>
-      </c>
-      <c r="C51" s="0" t="n">
-        <v>17267</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="0" t="n">
-        <v>8792</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="5" t="n">
-        <v>7063.86566162109</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G61" s="4"/>
-    </row>
-    <row r="62" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G62" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G63" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G64" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G65" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G66" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="L66" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="176.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="I67" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G68" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G69" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G70" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G71" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G72" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-    </row>
-    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G73" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G74" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G75" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I78" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I79" s="0" t="s">
-        <v>306</v>
-      </c>
-    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H6:I20"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E6:E19">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFE67C73"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="L66" r:id="rId1" display="*http://citeseerx.ist.psu.edu/viewdoc/summary?doi=10.1.1.686.2543"/>
+    <hyperlink ref="J6" r:id="rId1" display="(1)https://github.com/SonarSource/sonar-java/tree/ab10b6ecfaa502b96d314c66d0862714acbe400a/java-frontend/src/main/java/org/sonar/java/ast/visitors"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7480,4 +7616,917 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I138"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>69000</v>
+      </c>
+      <c r="D7" s="27" t="n">
+        <v>88113</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>25353.4317016602</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>48.6373901367188</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="27" t="n">
+        <v>88113</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>767.946243286133</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>18.1198120117188</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>104000</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>112000</v>
+      </c>
+      <c r="D9" s="27" t="n">
+        <v>88113</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1390.21873474121</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>41.0079956054687</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>284000</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>199000</v>
+      </c>
+      <c r="D10" s="27" t="n">
+        <v>88113</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>157000</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>226000</v>
+      </c>
+      <c r="D11" s="27" t="n">
+        <v>88113</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>191175.222396851</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>6941.31851196289</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>184000</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>157000</v>
+      </c>
+      <c r="D12" s="27" t="n">
+        <v>88113</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>6822.10922241211</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>238.656997680664</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>409.603118896484</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>18.8350677490234</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>41000</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>23000</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>90000</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>74000</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>281000</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>179000</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>12789.7262573242</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>382.184982299805</v>
+      </c>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>401000</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>267000</v>
+      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>11418.1041717529</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>382.184982299805</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">SUM(B7:B20)</f>
+        <v>1649000</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <f aca="false">SUM(C7:C20)</f>
+        <v>1317000</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">D7</f>
+        <v>88113</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">SUM(E7:E20)</f>
+        <v>250126.361846924</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">SUM(F7:F20)</f>
+        <v>8070.94573974609</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">B22/1000</f>
+        <v>1649</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <f aca="false">C22/1000</f>
+        <v>1317</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">D22/1000</f>
+        <v>88.113</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">E22/1000</f>
+        <v>250.126361846924</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">F22/1000</f>
+        <v>8.07094573974609</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">B23/1000</f>
+        <v>1.649</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">C23/1000</f>
+        <v>1.317</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">D23/1000</f>
+        <v>0.088113</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">E23/1000</f>
+        <v>0.250126361846924</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">F23/1000</f>
+        <v>0.00807094573974609</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="E33" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="F34" s="24"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>6450999.99999999</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>23792.2668457031</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>869.035720825195</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>5349000</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1071.45309448242</v>
+      </c>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>13083000</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>38703000</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>186646.223068237</v>
+      </c>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>9884000</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>6792.30690002441</v>
+      </c>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>31000</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>308.990478515625</v>
+      </c>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1816000</v>
+      </c>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>4906000</v>
+      </c>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>145000</v>
+      </c>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>13322000</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>11065.9599304199</v>
+      </c>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>19803000</v>
+      </c>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>12943.5062408447</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <f aca="false">SUM(B35:B48)</f>
+        <v>113575000</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <f aca="false">SUM(C35:C48)</f>
+        <v>243489.742279053</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <f aca="false">B50/1000</f>
+        <v>113575</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <f aca="false">C50/1000</f>
+        <v>243.489742279053</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <f aca="false">B51/1000</f>
+        <v>113.575</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <f aca="false">C51/1000</f>
+        <v>0.243489742279053</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C58" s="21"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>1588000</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>2877.95066833496</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>184.535980224609</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>2077000</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>430.583953857422</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>5520000</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>16078000</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>61530.1132202149</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>4926000</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>2512.93182373047</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>129.461288452148</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>2207000</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>1937000</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>5557000</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>5188.7035369873</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>7896000</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>4721.64154052734</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <f aca="false">SUM(B60:B73)</f>
+        <v>47876000</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <f aca="false">SUM(C60:C73)</f>
+        <v>77575.9220123291</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <f aca="false">B75/1000</f>
+        <v>47876</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <f aca="false">C75/1000</f>
+        <v>77.5759220123291</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <f aca="false">B76/1000</f>
+        <v>47.876</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <f aca="false">C76/1000</f>
+        <v>0.0775759220123291</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="7"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="H7:I21"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E34:F48"/>
+    <mergeCell ref="B58:C58"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>